<commit_message>
added 5 problems of recursion
</commit_message>
<xml_diff>
--- a/DSA 90 day.xlsx
+++ b/DSA 90 day.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gouri\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gouri\DSApractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288F64A2-BF21-4B3F-BABB-64E4F88FDB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC337910-CF4F-484F-B8C9-4EB20470182C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -229,6 +229,12 @@
                 <c:pt idx="18">
                   <c:v>45837</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>45838</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45839</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -294,6 +300,12 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -730,7 +742,7 @@
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -958,10 +970,26 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2">
+        <v>45838</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>13</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="2">
+        <v>45839</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>14</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>

</xml_diff>

<commit_message>
added letter combinations of a phone number
</commit_message>
<xml_diff>
--- a/DSA 90 day.xlsx
+++ b/DSA 90 day.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gouri\DSApractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC337910-CF4F-484F-B8C9-4EB20470182C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54754E4-EACE-4DE8-8724-57CA208B52D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -235,6 +235,9 @@
                 <c:pt idx="20">
                   <c:v>45839</c:v>
                 </c:pt>
+                <c:pt idx="21">
+                  <c:v>45840</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -306,6 +309,9 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -742,7 +748,7 @@
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -992,7 +998,15 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="2">
+        <v>45840</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>15</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>

</xml_diff>

<commit_message>
added count subarrays with sum divisible by k
</commit_message>
<xml_diff>
--- a/DSA 90 day.xlsx
+++ b/DSA 90 day.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gouri\DSApractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D58ABA-FAEA-4A8F-8E8F-ECE96D667D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDB48E7-7CB8-40E3-9EE8-6C0A65482823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Dates</t>
   </si>
@@ -40,6 +41,30 @@
   </si>
   <si>
     <t>cumulative progress</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>DSA</t>
+  </si>
+  <si>
+    <t>Web Dev</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t>MYSQL</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>days</t>
   </si>
 </sst>
 </file>
@@ -80,10 +105,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,7 +797,7 @@
   </sheetPr>
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1302,4 +1328,95 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54CC812-8662-4A10-840B-1BB67D4E9C58}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3">
+        <v>45819</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45930</v>
+      </c>
+      <c r="F3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45931</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45961</v>
+      </c>
+      <c r="F5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
+        <v>45962</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45976</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>45977</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45991</v>
+      </c>
+      <c r="F9">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>